<commit_message>
addet modifide fille ad-hoc.xlsx
</commit_message>
<xml_diff>
--- a/ad-hoc.xlsx
+++ b/ad-hoc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Чек-лист" sheetId="1" r:id="rId1"/>
@@ -14,14 +14,19 @@
     <sheet name="Bug report 4" sheetId="5" r:id="rId5"/>
     <sheet name="Bug report 5" sheetId="6" r:id="rId6"/>
     <sheet name="мобільний додакток " sheetId="7" r:id="rId7"/>
-    <sheet name="Лист2" sheetId="8" r:id="rId8"/>
+    <sheet name="Приклад 1" sheetId="8" r:id="rId8"/>
+    <sheet name="Приклад 2" sheetId="9" r:id="rId9"/>
+    <sheet name="Приклад 3" sheetId="10" r:id="rId10"/>
+    <sheet name="Приклад 4" sheetId="11" r:id="rId11"/>
+    <sheet name="Приклад 5" sheetId="12" r:id="rId12"/>
+    <sheet name="Приклад 6" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="211">
   <si>
     <t>Коментар</t>
   </si>
@@ -537,9 +542,6 @@
     <t>Реєстрація (за номером телефону/через соц. мережі/e-mail)</t>
   </si>
   <si>
-    <t>Онбординг нових користувачів</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Валідація обов'язкових полів</t>
   </si>
   <si>
@@ -558,12 +560,6 @@
     <t xml:space="preserve"> Бонуси</t>
   </si>
   <si>
-    <t xml:space="preserve"> Коректне відображення помилок</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Робота з файлами (надсилання/отримання/перегляд)</t>
-  </si>
-  <si>
     <t>Скролл/свайп елементів</t>
   </si>
   <si>
@@ -591,9 +587,6 @@
     <t xml:space="preserve"> Інформація про операції (чеки і т.д.)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Різні способи оплати (Google Pay, Apple Pay)</t>
-  </si>
-  <si>
     <t>Тестування датчиків (освітленості, температури пристрою, гіроскоп тощо)</t>
   </si>
   <si>
@@ -609,9 +602,6 @@
     <t xml:space="preserve"> Тексти захищені всередині програми та користувач в налаштуваннях програми може виставити необхідну мову</t>
   </si>
   <si>
-    <t>Тексти залежать від мови у системних налаштуваннях</t>
-  </si>
-  <si>
     <t>Коректне відображення елементів на пристроях з різною роздільною здатністю екранів</t>
   </si>
   <si>
@@ -630,88 +620,121 @@
     <t>Посилання на документи ведуть на відповідний розділ</t>
   </si>
   <si>
-    <t xml:space="preserve"> Анімація між переходами</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Коректне повернення на попередній екран</t>
   </si>
   <si>
     <t xml:space="preserve"> Підтримуються основні жести під час роботи із сенсорними екранами (swipe back тощо.)</t>
   </si>
   <si>
-    <t>Високе завантаження центрального процесора</t>
-  </si>
-  <si>
-    <t>Нестача пам'яті</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Завантаження батареї</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Відмови</t>
-  </si>
-  <si>
-    <t>Низька пропускна спроможність мережі</t>
-  </si>
-  <si>
-    <t>Працездатність програми на різних пристроях різних виробників</t>
-  </si>
-  <si>
-    <t>Час завантаження програми</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Обробка запитів</t>
-  </si>
-  <si>
-    <t>Кешування даних</t>
-  </si>
-  <si>
-    <t>Споживання ресурсів програмою (наприклад витрата заряду батареї)</t>
-  </si>
-  <si>
-    <t>Функціональне тестування</t>
-  </si>
-  <si>
     <t>Шарінг контенту в соц. мережі</t>
   </si>
   <si>
-    <t>Політики конфіденційності та інші посилання на документи</t>
-  </si>
-  <si>
-    <t>Тестування дозволів (доступ до камери/мікрофону/галереї/і т.д.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Дані користувача (паролі) не передаються у відкритому вигляді</t>
-  </si>
-  <si>
-    <t>У полях, з введенням пароля та підтвердженням пароля, дані ховаються астерисками</t>
-  </si>
-  <si>
-    <t>функція відсутня</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Профіль відсутній </t>
-  </si>
-  <si>
-    <t>Відсутні сповіщення</t>
-  </si>
-  <si>
-    <t>Spaceflight simulator v 1.5.9.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Відсутня функція </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Реєстрація через google аккаунт </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Велика кількість взаємодій користувача з програмою </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Відсутні </t>
-  </si>
-  <si>
     <t>Чек лист ad-hoc тестування</t>
+  </si>
+  <si>
+    <t>ad-hoc  тестування</t>
+  </si>
+  <si>
+    <t>Megogo V:4.7.9</t>
+  </si>
+  <si>
+    <t>xiaomi redmi 10 MIUI global 13.05.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Наявність угоди користувача </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Перевірка на кросплатформенімть </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Можливість бесплатного перегляду </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Можливість вибору підписки </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Увесь контент розподілений за жанрами </t>
+  </si>
+  <si>
+    <t>Присутній відео контент</t>
+  </si>
+  <si>
+    <t>Присутній аудіо контент</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Увесь контент розподілений за катигоріями </t>
+  </si>
+  <si>
+    <t>Функція обране</t>
+  </si>
+  <si>
+    <t>Функція продовжити перегляд</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Функція перегляду телеканалів </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Функція перегляду каналів у реальному часі </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Доступ до перегляду у два тижні </t>
+  </si>
+  <si>
+    <t>Функція перегляду каналів у минулому часі</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Присутні </t>
+  </si>
+  <si>
+    <t xml:space="preserve">При згортанні програми під час перегляду створюється зменшиний єкран у низу єкрану телефону </t>
+  </si>
+  <si>
+    <t>працює стабільно</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Доступ до акаунті з інших пристроїв </t>
+  </si>
+  <si>
+    <t>Приклад 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Різні способи оплати </t>
+  </si>
+  <si>
+    <t>Функція повернення в ефір</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Завантаження мережі при WI/FI зв'язку  (застосунок у фоновому режимі якість відео "Авто") </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Завантаження мережі при стільниковому зв'язку (застосунок у фоновому режимі якість відео "Авто") </t>
+  </si>
+  <si>
+    <t>Приклад 2</t>
+  </si>
+  <si>
+    <t>Приклад 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Завантаження мережі при стільниковому зв'язку (застосунок у фоновому режиміякість відео"1080" ) Перевірка після згортання </t>
+  </si>
+  <si>
+    <t>Приклад 4'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Завантаження мережі при WI/FI зв'язку (застосунок у фоновому режиміякість відео"1080" ) Перевірка після згортання </t>
+  </si>
+  <si>
+    <t>Приклад 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Навантаження на батарею </t>
+  </si>
+  <si>
+    <t>Приклад 6</t>
+  </si>
+  <si>
+    <t>Android , Windows (Google chrome / Версия 111.0.5563.147 (Официальная сборка), (64 бит) , Tizen.</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1031,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1095,6 +1118,7 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1134,6 +1158,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1188,6 +1224,49 @@
         <a:xfrm>
           <a:off x="3467100" y="11001375"/>
           <a:ext cx="6430272" cy="3000794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>524544</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>67961</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="762000"/>
+          <a:ext cx="4791744" cy="9211961"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1393,6 +1472,594 @@
         <a:xfrm>
           <a:off x="4953000" y="12963524"/>
           <a:ext cx="4086226" cy="1323975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>134075</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>172617</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="428625" y="0"/>
+          <a:ext cx="5191850" cy="8364117"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Прямая со стрелкой 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3800475" y="2428876"/>
+          <a:ext cx="2638425" cy="942974"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Скругленный прямоугольник 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6296025" y="2000250"/>
+          <a:ext cx="4162425" cy="809625"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6477000" y="2152650"/>
+          <a:ext cx="3724275" cy="476250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="uk-UA" sz="1600"/>
+            <a:t>Україньська</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="uk-UA" sz="1600" baseline="0"/>
+            <a:t> версія </a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>296082</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>39328</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Рисунок 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="9334500"/>
+          <a:ext cx="5782482" cy="8802328"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Прямая со стрелкой 13"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3952876" y="12001500"/>
+          <a:ext cx="2971799" cy="1276350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Скругленный прямоугольник 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7029450" y="11258550"/>
+          <a:ext cx="3867150" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="TextBox 16"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7239000" y="11372850"/>
+          <a:ext cx="3409950" cy="581025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1600"/>
+            <a:t>Російська версія</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>486400</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>125145</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="276225" y="0"/>
+          <a:ext cx="4477375" cy="9459645"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>162543</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>134671</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="571500"/>
+          <a:ext cx="4429743" cy="9469171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>86335</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>115576</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="590550" y="114300"/>
+          <a:ext cx="4372585" cy="9145276"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>315050</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>144171</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="381000"/>
+          <a:ext cx="5191850" cy="9288171"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1693,7 +2360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -1705,28 +2372,28 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="36" t="s">
-        <v>204</v>
-      </c>
-      <c r="D6" s="37"/>
+      <c r="C6" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="38"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
         <v>0</v>
@@ -2229,7 +2896,7 @@
       <c r="E45" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="39" t="s">
+      <c r="F45" s="40" t="s">
         <v>126</v>
       </c>
       <c r="G45" s="23"/>
@@ -2244,7 +2911,7 @@
       <c r="E46" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="40"/>
+      <c r="F46" s="41"/>
       <c r="G46" s="23"/>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.25">
@@ -2257,7 +2924,7 @@
       <c r="E47" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="40"/>
+      <c r="F47" s="41"/>
       <c r="G47" s="23"/>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.25">
@@ -2270,7 +2937,7 @@
       <c r="E48" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="40"/>
+      <c r="F48" s="41"/>
       <c r="G48" s="23"/>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.25">
@@ -2283,7 +2950,7 @@
       <c r="E49" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F49" s="40"/>
+      <c r="F49" s="41"/>
       <c r="G49" s="23"/>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.25">
@@ -2296,7 +2963,7 @@
       <c r="E50" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="40"/>
+      <c r="F50" s="41"/>
       <c r="G50" s="23"/>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.25">
@@ -2309,7 +2976,7 @@
       <c r="E51" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F51" s="40"/>
+      <c r="F51" s="41"/>
       <c r="G51" s="23"/>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
@@ -2322,7 +2989,7 @@
       <c r="E52" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F52" s="40"/>
+      <c r="F52" s="41"/>
       <c r="G52" s="23"/>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.25">
@@ -2335,7 +3002,7 @@
       <c r="E53" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F53" s="40"/>
+      <c r="F53" s="41"/>
       <c r="G53" s="23"/>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.25">
@@ -2348,7 +3015,7 @@
       <c r="E54" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F54" s="40"/>
+      <c r="F54" s="41"/>
       <c r="G54" s="23"/>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.25">
@@ -2361,7 +3028,7 @@
       <c r="E55" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="40"/>
+      <c r="F55" s="41"/>
       <c r="G55" s="23"/>
     </row>
     <row r="56" spans="3:7" ht="30" x14ac:dyDescent="0.25">
@@ -2374,7 +3041,7 @@
       <c r="E56" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F56" s="40"/>
+      <c r="F56" s="41"/>
       <c r="G56" s="23"/>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.25">
@@ -2387,14 +3054,14 @@
       <c r="E57" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F57" s="41"/>
+      <c r="F57" s="42"/>
       <c r="G57" s="23"/>
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C73" s="38"/>
-      <c r="D73" s="38"/>
-      <c r="E73" s="38"/>
-      <c r="F73" s="38"/>
+      <c r="C73" s="39"/>
+      <c r="D73" s="39"/>
+      <c r="E73" s="39"/>
+      <c r="F73" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2415,12 +3082,64 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C30"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2430,10 +3149,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="42"/>
+      <c r="C3" s="43"/>
     </row>
     <row r="4" spans="2:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
@@ -2444,16 +3163,16 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="44" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
     </row>
     <row r="7" spans="2:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
@@ -2512,10 +3231,10 @@
       </c>
     </row>
     <row r="14" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="44"/>
+      <c r="C14" s="45"/>
     </row>
     <row r="15" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
@@ -2534,16 +3253,16 @@
       </c>
     </row>
     <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="44"/>
+      <c r="C17" s="45"/>
     </row>
     <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="46" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2551,7 +3270,7 @@
       <c r="B19" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="46"/>
+      <c r="C19" s="47"/>
     </row>
     <row r="20" spans="2:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="14">
@@ -2589,7 +3308,7 @@
       <c r="B24" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="43" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2597,13 +3316,13 @@
       <c r="B25" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="42"/>
+      <c r="C25" s="43"/>
     </row>
     <row r="26" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="43" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2611,25 +3330,25 @@
       <c r="B27" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="42"/>
+      <c r="C27" s="43"/>
     </row>
     <row r="28" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="42"/>
+      <c r="C28" s="43"/>
     </row>
     <row r="29" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="42"/>
+      <c r="C29" s="43"/>
     </row>
     <row r="30" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C30" s="42"/>
+      <c r="C30" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2666,10 +3385,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="42"/>
+      <c r="D4" s="43"/>
     </row>
     <row r="5" spans="3:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
@@ -2680,16 +3399,16 @@
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="44" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
     </row>
     <row r="8" spans="3:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="14" t="s">
@@ -2748,10 +3467,10 @@
       </c>
     </row>
     <row r="15" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="44"/>
+      <c r="D15" s="45"/>
     </row>
     <row r="16" spans="3:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="14" t="s">
@@ -2770,16 +3489,16 @@
       </c>
     </row>
     <row r="18" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="44"/>
+      <c r="D18" s="45"/>
     </row>
     <row r="19" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C19" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="45" t="s">
+      <c r="D19" s="46" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2787,7 +3506,7 @@
       <c r="C20" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="46"/>
+      <c r="D20" s="47"/>
     </row>
     <row r="21" spans="3:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="14">
@@ -2841,7 +3560,7 @@
       <c r="C27" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="43" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2849,13 +3568,13 @@
       <c r="C28" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="42"/>
+      <c r="D28" s="43"/>
     </row>
     <row r="29" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C29" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="43" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2863,25 +3582,25 @@
       <c r="C30" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="42"/>
+      <c r="D30" s="43"/>
     </row>
     <row r="31" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C31" s="42" t="s">
+      <c r="C31" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="42"/>
+      <c r="D31" s="43"/>
     </row>
     <row r="32" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C32" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="42"/>
+      <c r="D32" s="43"/>
     </row>
     <row r="33" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C33" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="42"/>
+      <c r="D33" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2919,10 +3638,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="D4" s="42"/>
+      <c r="D4" s="43"/>
     </row>
     <row r="5" spans="3:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
@@ -2933,16 +3652,16 @@
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="44" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
     </row>
     <row r="8" spans="3:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="14" t="s">
@@ -3001,10 +3720,10 @@
       </c>
     </row>
     <row r="15" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="44"/>
+      <c r="D15" s="45"/>
     </row>
     <row r="16" spans="3:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="14" t="s">
@@ -3023,16 +3742,16 @@
       </c>
     </row>
     <row r="18" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="44"/>
+      <c r="D18" s="45"/>
     </row>
     <row r="19" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C19" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="45" t="s">
+      <c r="D19" s="46" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3040,7 +3759,7 @@
       <c r="C20" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="46"/>
+      <c r="D20" s="47"/>
     </row>
     <row r="21" spans="3:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="14">
@@ -3078,7 +3797,7 @@
       <c r="C25" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="42" t="s">
+      <c r="D25" s="43" t="s">
         <v>106</v>
       </c>
     </row>
@@ -3086,13 +3805,13 @@
       <c r="C26" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="42"/>
+      <c r="D26" s="43"/>
     </row>
     <row r="27" spans="3:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="43" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3100,25 +3819,25 @@
       <c r="C28" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="42"/>
+      <c r="D28" s="43"/>
     </row>
     <row r="29" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="D29" s="42"/>
+      <c r="D29" s="43"/>
     </row>
     <row r="30" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C30" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="42"/>
+      <c r="D30" s="43"/>
     </row>
     <row r="31" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C31" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="42"/>
+      <c r="D31" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3156,10 +3875,10 @@
   </cols>
   <sheetData>
     <row r="7" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="42"/>
+      <c r="C7" s="43"/>
     </row>
     <row r="8" spans="2:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
@@ -3170,16 +3889,16 @@
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="44" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
     </row>
     <row r="11" spans="2:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
@@ -3238,10 +3957,10 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="44"/>
+      <c r="C18" s="45"/>
     </row>
     <row r="19" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
@@ -3260,16 +3979,16 @@
       </c>
     </row>
     <row r="21" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="44"/>
+      <c r="C21" s="45"/>
     </row>
     <row r="22" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="45" t="s">
+      <c r="C22" s="46" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3277,7 +3996,7 @@
       <c r="B23" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="46"/>
+      <c r="C23" s="47"/>
     </row>
     <row r="24" spans="2:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="14">
@@ -3373,7 +4092,7 @@
       <c r="B35" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="42" t="s">
+      <c r="C35" s="43" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3381,13 +4100,13 @@
       <c r="B36" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="42"/>
+      <c r="C36" s="43"/>
     </row>
     <row r="37" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B37" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="42" t="s">
+      <c r="C37" s="43" t="s">
         <v>116</v>
       </c>
     </row>
@@ -3395,25 +4114,25 @@
       <c r="B38" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="42"/>
+      <c r="C38" s="43"/>
     </row>
     <row r="39" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="42"/>
+      <c r="C39" s="43"/>
     </row>
     <row r="40" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B40" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="42"/>
+      <c r="C40" s="43"/>
     </row>
     <row r="41" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="42"/>
+      <c r="C41" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3441,7 +4160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
@@ -3452,10 +4171,10 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="42"/>
+      <c r="D5" s="43"/>
     </row>
     <row r="6" spans="3:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="14" t="s">
@@ -3466,16 +4185,16 @@
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="44" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
     </row>
     <row r="9" spans="3:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="14" t="s">
@@ -3534,10 +4253,10 @@
       </c>
     </row>
     <row r="16" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="44"/>
+      <c r="D16" s="45"/>
     </row>
     <row r="17" spans="3:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="14" t="s">
@@ -3556,16 +4275,16 @@
       </c>
     </row>
     <row r="19" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="44"/>
+      <c r="D19" s="45"/>
     </row>
     <row r="20" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C20" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="45" t="s">
+      <c r="D20" s="46" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3573,7 +4292,7 @@
       <c r="C21" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="46"/>
+      <c r="D21" s="47"/>
     </row>
     <row r="22" spans="3:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="14">
@@ -3595,7 +4314,7 @@
       <c r="C24" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="47" t="s">
+      <c r="D24" s="48" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3603,13 +4322,13 @@
       <c r="C25" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="47"/>
+      <c r="D25" s="48"/>
     </row>
     <row r="26" spans="3:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="42" t="s">
+      <c r="D26" s="43" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3617,25 +4336,25 @@
       <c r="C27" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="42"/>
+      <c r="D27" s="43"/>
     </row>
     <row r="28" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="42"/>
+      <c r="D28" s="43"/>
     </row>
     <row r="29" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C29" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="42"/>
+      <c r="D29" s="43"/>
     </row>
     <row r="30" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C30" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="42"/>
+      <c r="D30" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3662,8 +4381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K59"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView topLeftCell="B29" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3673,16 +4392,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" s="27" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:10" s="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="27" t="s">
+        <v>178</v>
+      </c>
+    </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B5" s="30"/>
       <c r="C5" s="31" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="33" t="s">
@@ -3711,17 +4434,19 @@
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>143</v>
+        <v>180</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>210</v>
+      </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
@@ -3733,14 +4458,12 @@
         <v>3</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>201</v>
-      </c>
+      <c r="E8" s="4"/>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
@@ -3752,14 +4475,12 @@
         <v>4</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>201</v>
-      </c>
+      <c r="E9" s="4"/>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
@@ -3771,14 +4492,12 @@
         <v>5</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>196</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
@@ -3790,7 +4509,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>1</v>
@@ -3807,7 +4526,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>1</v>
@@ -3824,26 +4543,24 @@
         <v>8</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>197</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4"/>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>9</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>150</v>
+        <v>179</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>1</v>
@@ -3860,7 +4577,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>1</v>
@@ -3877,7 +4594,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>1</v>
@@ -3894,7 +4611,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>1</v>
@@ -3911,7 +4628,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>154</v>
+        <v>181</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>1</v>
@@ -3923,12 +4640,12 @@
       <c r="I18" s="28"/>
       <c r="J18" s="28"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <v>14</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>1</v>
@@ -3940,31 +4657,29 @@
       <c r="I19" s="28"/>
       <c r="J19" s="28"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>15</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>198</v>
-      </c>
+      <c r="E20" s="4"/>
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
       <c r="I20" s="28"/>
       <c r="J20" s="28"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
         <v>16</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>1</v>
@@ -3976,12 +4691,12 @@
       <c r="I21" s="28"/>
       <c r="J21" s="28"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
         <v>17</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>158</v>
+        <v>184</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>1</v>
@@ -3993,12 +4708,12 @@
       <c r="I22" s="28"/>
       <c r="J22" s="28"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
         <v>18</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>159</v>
+        <v>185</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>1</v>
@@ -4010,12 +4725,12 @@
       <c r="I23" s="28"/>
       <c r="J23" s="28"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <v>19</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>160</v>
+        <v>187</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>1</v>
@@ -4027,12 +4742,12 @@
       <c r="I24" s="28"/>
       <c r="J24" s="28"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
         <v>20</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>161</v>
+        <v>188</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>1</v>
@@ -4044,67 +4759,65 @@
       <c r="I25" s="28"/>
       <c r="J25" s="28"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
         <v>21</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>200</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4"/>
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
       <c r="J26" s="28"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <v>22</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>200</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="4"/>
       <c r="F27" s="28"/>
       <c r="G27" s="28"/>
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
       <c r="J27" s="28"/>
     </row>
-    <row r="28" spans="2:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
         <v>23</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="4"/>
+      <c r="D28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>191</v>
+      </c>
       <c r="F28" s="28"/>
       <c r="G28" s="28"/>
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
       <c r="J28" s="28"/>
     </row>
-    <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <v>24</v>
       </c>
-      <c r="C29" s="29" t="s">
-        <v>163</v>
+      <c r="C29" s="4" t="s">
+        <v>199</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>1</v>
@@ -4113,13 +4826,15 @@
       <c r="F29" s="28"/>
       <c r="G29" s="28"/>
       <c r="H29" s="28"/>
-    </row>
-    <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="4">
         <v>25</v>
       </c>
-      <c r="C30" s="29" t="s">
-        <v>164</v>
+      <c r="C30" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>1</v>
@@ -4128,296 +4843,346 @@
       <c r="F30" s="28"/>
       <c r="G30" s="28"/>
       <c r="H30" s="28"/>
-    </row>
-    <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
         <v>26</v>
       </c>
-      <c r="C31" s="29" t="s">
-        <v>165</v>
+      <c r="C31" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>193</v>
+      </c>
       <c r="F31" s="28"/>
       <c r="G31" s="28"/>
       <c r="H31" s="28"/>
-    </row>
-    <row r="32" spans="2:10" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+    </row>
+    <row r="32" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="4">
         <v>27</v>
       </c>
-      <c r="C32" s="29" t="s">
-        <v>166</v>
+      <c r="C32" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>194</v>
+      </c>
       <c r="F32" s="28"/>
       <c r="G32" s="28"/>
       <c r="H32" s="28"/>
-    </row>
-    <row r="33" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
         <v>28</v>
       </c>
-      <c r="C33" s="29" t="s">
-        <v>167</v>
+      <c r="C33" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>195</v>
+      </c>
       <c r="F33" s="28"/>
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
-    </row>
-    <row r="34" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
+    </row>
+    <row r="34" spans="2:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="4">
         <v>29</v>
       </c>
-      <c r="C34" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34" s="4"/>
-      <c r="F34" s="28"/>
+      <c r="C34" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="49" t="s">
+        <v>203</v>
+      </c>
+      <c r="F34" s="50"/>
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
       <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
-    </row>
-    <row r="35" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:10" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="4">
         <v>30</v>
       </c>
-      <c r="C35" s="29" t="s">
-        <v>169</v>
+      <c r="C35" s="4" t="s">
+        <v>201</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="28"/>
+      <c r="E35" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="F35" s="50"/>
       <c r="G35" s="28"/>
       <c r="H35" s="28"/>
       <c r="I35" s="28"/>
       <c r="J35" s="28"/>
-      <c r="K35" s="28"/>
-    </row>
-    <row r="36" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:10" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="4">
         <v>31</v>
       </c>
-      <c r="C36" s="29" t="s">
-        <v>170</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="28"/>
+      <c r="C36" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="F36" s="50"/>
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
       <c r="I36" s="28"/>
       <c r="J36" s="28"/>
-      <c r="K36" s="28"/>
-    </row>
-    <row r="37" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="2:10" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="4">
         <v>32</v>
       </c>
-      <c r="C37" s="29" t="s">
-        <v>171</v>
+      <c r="C37" s="4" t="s">
+        <v>206</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="28"/>
+      <c r="E37" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="F37" s="50"/>
       <c r="G37" s="28"/>
       <c r="H37" s="28"/>
       <c r="I37" s="28"/>
       <c r="J37" s="28"/>
-      <c r="K37" s="28"/>
-    </row>
-    <row r="38" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="2:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="4">
         <v>33</v>
       </c>
-      <c r="C38" s="29" t="s">
-        <v>172</v>
+      <c r="C38" s="4" t="s">
+        <v>208</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E38" s="52" t="s">
+        <v>209</v>
+      </c>
+      <c r="F38" s="50"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="4">
         <v>34</v>
       </c>
-      <c r="C39" s="29" t="s">
-        <v>173</v>
+      <c r="C39" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="28"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="4">
         <v>35</v>
       </c>
-      <c r="C40" s="29" t="s">
-        <v>174</v>
+      <c r="C40" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E40" s="4"/>
-    </row>
-    <row r="41" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="28"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="4">
         <v>36</v>
       </c>
-      <c r="C41" s="29" t="s">
-        <v>175</v>
+      <c r="C41" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E41" s="4"/>
-    </row>
-    <row r="42" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="28"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="4">
         <v>37</v>
       </c>
-      <c r="C42" s="29" t="s">
-        <v>176</v>
+      <c r="C42" s="4" t="s">
+        <v>174</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="4">
         <v>38</v>
       </c>
-      <c r="C43" s="29" t="s">
-        <v>177</v>
+      <c r="C43" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F43" s="28"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="28"/>
+    </row>
+    <row r="44" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="4">
         <v>39</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E44" s="4"/>
-    </row>
-    <row r="45" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
+    </row>
+    <row r="45" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="4">
         <v>40</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E45" s="4"/>
-    </row>
-    <row r="46" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+    </row>
+    <row r="46" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="4">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="D46" s="4"/>
+        <v>161</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E46" s="4"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
       <c r="H46" s="28"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="28"/>
-      <c r="K46" s="28"/>
-    </row>
-    <row r="47" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="2:10" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B47" s="4">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>181</v>
-      </c>
-      <c r="D47" s="4"/>
+        <v>162</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E47" s="4"/>
       <c r="F47" s="28"/>
       <c r="G47" s="28"/>
       <c r="H47" s="28"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="28"/>
-      <c r="K47" s="28"/>
-    </row>
-    <row r="48" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="4">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="D48" s="4"/>
+        <v>163</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E48" s="4"/>
       <c r="F48" s="28"/>
       <c r="G48" s="28"/>
       <c r="H48" s="28"/>
-      <c r="I48" s="28"/>
-      <c r="J48" s="28"/>
-      <c r="K48" s="28"/>
-    </row>
-    <row r="49" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="2:11" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="4">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C49" s="29" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E49" s="4" t="s">
-        <v>203</v>
-      </c>
+      <c r="E49" s="4"/>
       <c r="F49" s="28"/>
       <c r="G49" s="28"/>
       <c r="H49" s="28"/>
-      <c r="I49" s="28"/>
-      <c r="J49" s="28"/>
-      <c r="K49" s="28"/>
     </row>
     <row r="50" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="4">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C50" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="D50" s="4"/>
+        <v>164</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E50" s="4"/>
       <c r="F50" s="28"/>
       <c r="G50" s="28"/>
@@ -4426,58 +5191,74 @@
       <c r="J50" s="28"/>
       <c r="K50" s="28"/>
     </row>
-    <row r="51" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B51" s="4">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C51" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="28"/>
+        <v>165</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" s="51" t="s">
+        <v>197</v>
+      </c>
+      <c r="F51" s="50"/>
       <c r="G51" s="28"/>
       <c r="H51" s="28"/>
       <c r="I51" s="28"/>
       <c r="J51" s="28"/>
       <c r="K51" s="28"/>
     </row>
-    <row r="52" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B52" s="4">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>185</v>
-      </c>
-      <c r="D52" s="4"/>
+        <v>166</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E52" s="4"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="28"/>
+      <c r="J52" s="28"/>
+      <c r="K52" s="28"/>
     </row>
     <row r="53" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="4">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C53" s="29" t="s">
-        <v>186</v>
-      </c>
-      <c r="D53" s="4"/>
+        <v>167</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E53" s="4"/>
     </row>
     <row r="54" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="4">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>187</v>
-      </c>
-      <c r="D54" s="4"/>
+        <v>168</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E54" s="4"/>
     </row>
     <row r="55" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="4">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>1</v>
@@ -4486,45 +5267,61 @@
     </row>
     <row r="56" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="4">
+        <v>51</v>
+      </c>
+      <c r="C56" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B57" s="4">
         <v>52</v>
       </c>
-      <c r="C56" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-    </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="4">
+      <c r="C57" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B58" s="4">
         <v>53</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-    </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B58" s="4">
+      <c r="C58" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="B59" s="4">
         <v>54</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-    </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="4">
-        <v>55</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
+      <c r="C59" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E59" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E51" location="'Приклад 1'!A1" display="Приклад 1"/>
+    <hyperlink ref="E38" location="'Приклад 6'!A1" display="Приклад 6"/>
+    <hyperlink ref="E37" location="'Приклад 5'!A1" display="Приклад 5"/>
+    <hyperlink ref="E36" location="'Приклад 4'!A1" display="Приклад 4'"/>
+    <hyperlink ref="E34" location="'Приклад 3'!A1" display="Приклад 3"/>
+    <hyperlink ref="E35" location="'Приклад 2'!A1" display="Приклад 2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4534,10 +5331,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>